<commit_message>
chore: Update `ontology_definition.xlsx` and add `.DS_Store` files.
</commit_message>
<xml_diff>
--- a/backend/ontology_definition.xlsx
+++ b/backend/ontology_definition.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,46 +447,220 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>dcat:Catalog</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>dcat:Dataset</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>dcat:Resource</t>
-        </is>
-      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Dataset</t>
+          <t>Catalog</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>A collection of data, published or curated by a single agent.</t>
+          <t>A curated collection of metadata about resources (e.g., datasets and data services in the context of a data catalog).</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ext:HealthDataset</t>
+          <t>dcat:CatalogRecord</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>n9ab3b25b15354447951569b746ff58f2b18</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Catalog Record</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>A record in a data catalog, describing the registration of a single dataset or data service.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>dcat:DataService</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>dctype:Service</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Data service</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>A site or end-point providing operations related to the discovery of, access to, or processing functions on, data or related resources.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>dcat:Dataset</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Health Dataset</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>A dataset containing health-related information.</t>
-        </is>
-      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>dcat:Resource</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>A collection of data, published or curated by a single source, and available for access or download in one or more representations.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>dcat:DatasetSeries</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>dcat:Dataset</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Dataset series</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>A collection of datasets that are published separately, but share some characteristics that group them.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>dcat:Distribution</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Distribution</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>A specific representation of a dataset. A dataset might be available in multiple serializations that may differ in various ways, including natural language, media-type or format, schematic organization, temporal and spatial resolution, level of detail or profiles (which might specify any or all of the above).</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>dcat:Relationship</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Relationship</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>An association class for attaching additional information to a relationship between DCAT Resources.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>dcat:Resource</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Catalogued resource</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Resource published or curated by a single agent.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>dcat:Role</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>skos:Concept</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Role</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>A role is the function of a resource or agent with respect to another resource, in the context of resource attribution or resource relationships.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ext:ConstructionProject</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>dcat:Resource</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Construction Project</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>A project related to the construction domain (Example).</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>n9ab3b25b15354447951569b746ff58f2b22</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -499,7 +673,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -547,64 +721,1003 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>dct:title</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>dcat:Dataset</t>
-        </is>
-      </c>
+          <t>dcat:accessService</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>xsd:string</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
+          <t>dcat:DataService</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Title</t>
+          <t>data access service</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>A name given to the dataset.</t>
+          <t>A site or end-point that gives access to the distribution of the dataset.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ext:patientCount</t>
+          <t>dcat:accessURL</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ext:HealthDataset</t>
+          <t>dcat:Distribution</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>xsd:integer</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1</v>
-      </c>
+          <t>rdfs:Resource</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Patient Count</t>
+          <t>access address</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Number of patients in the dataset.</t>
+          <t>A URL of a resource that gives access to a distribution of the dataset. E.g. landing page, feed, SPARQL endpoint. Use for all cases except a simple download link, in which case downloadURL is preferred.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>dcat:bbox</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>dcterms:Location</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>rdfs:Literal</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>bounding box</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>The geographic bounding box of a spatial thing [SDW-BP].</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>dcat:byteSize</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>dcat:Distribution</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>rdfs:Literal</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>byte size</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>The size of a distribution in bytes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>dcat:catalog</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>dcat:Catalog</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>dcat:Catalog</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>catalog</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>A catalog that is listed in the catalog.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>dcat:centroid</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>dcterms:Location</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>rdfs:Literal</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>centroid</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>The geographic center (centroid) of a spatial thing [SDW-BP].</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>dcat:compressFormat</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>dcat:Distribution</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>dcterms:MediaType</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>compression format</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>The compression format of the distribution in which the data is contained in a compressed form, e.g. to reduce the size of the downloadable file.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>dcat:contactPoint</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>vcard:Kind</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>contact point</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Relevant contact information for the catalogued resource. Use of vCard is recommended.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>dcat:dataset</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>dcat:Catalog</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>dcat:Dataset</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>dataset</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>A dataset that is listed in the catalog.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>dcat:distribution</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>dcat:Dataset</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>dcat:Distribution</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>distribution</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>An available distribution of the dataset.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>dcat:downloadURL</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>dcat:Distribution</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>rdfs:Resource</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>download URL</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>The URL of the downloadable file in a given format. E.g. CSV file or RDF file. The format is indicated by the distribution's dcterms:format and/or dcat:mediaType.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>dcat:endDate</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>dcterms:PeriodOfTime</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>rdfs:Literal</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>end date</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>The end of the period.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>dcat:endpointDescription</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>dcat:DataService</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>description of service end-point</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>A description of the service end-point, including its operations, parameters etc.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>dcat:endpointURL</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>dcat:DataService</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>rdfs:Resource</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>service end-point</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>The root location or primary endpoint of the service (a web-resolvable IRI).</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>dcat:first</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>first</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>The first resource in an ordered collection or series of resources, to which the current resource belongs.</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>dcat:hadRole</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>n9ab3b25b15354447951569b746ff58f2b22</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>dcat:Role</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>hadRole</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>The function of an entity or agent with respect to another entity or resource.</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>dcat:hasCurrentVersion</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>has current version</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>This resource has a more specific, versioned resource with equivalent content [PAV].</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>dcat:hasVersion</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>has version</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>This resource has a more specific, versioned resource [PAV].</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>dcat:inSeries</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>in series</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>A dataset series of which the dataset is part.</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>dcat:keyword</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>rdfs:Literal</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>keyword</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>A keyword or tag describing a resource.</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>dcat:landingPage</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>foaf:Document</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>landing page</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>A Web page that can be navigated to in a Web browser to gain access to the catalog, a dataset, its distributions and/or additional information.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>dcat:last</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>last</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>The last resource in an ordered collection or series of resources, to which the current resource belongs.</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>dcat:mediaType</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>dcat:Distribution</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>dcterms:MediaType</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>media type</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>The media type of the distribution as defined by IANA</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>dcat:packageFormat</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>dcat:Distribution</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>dcterms:MediaType</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>packaging format</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>The package format of the distribution in which one or more data files are grouped together, e.g. to enable a set of related files to be downloaded together.</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>dcat:prev</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>previous</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>The previous resource (before the current one) in an ordered collection or series of resources.</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>dcat:previousVersion</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>previous version</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>The previous version of a resource in a lineage [PAV].</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>dcat:qualifiedRelation</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>dcat:Resource</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>dcat:Relationship</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>qualified relation</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Link to a description of a relationship with another resource.</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>dcat:record</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>dcat:Catalog</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>dcat:CatalogRecord</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>record</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>A record describing the registration of a single dataset or data service that is part of the catalog.</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>dcat:resource</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>dcat:Catalog</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>dcat:Resource</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>resource</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>A resource that is listed in the catalog.</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>dcat:servesDataset</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>dcat:DataService</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>dcat:Dataset</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>serves dataset</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>A collection of data that this DataService can distribute.</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>dcat:service</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>dcat:Catalog</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>dcat:DataService</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>service</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>A service that is listed in the catalog.</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>dcat:spatialResolutionInMeters</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>xsd:decimal</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>prostorové rozlišení (metry)</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>minimum spatial separation resolvable in a dataset, measured in meters.</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>dcat:startDate</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>dcterms:PeriodOfTime</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>rdfs:Literal</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>start date</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>dcat:temporalResolution</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>xsd:duration</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>temporal resolution</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>minimum time period resolvable in a dataset.</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>dcat:theme</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>theme</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>A main category of the resource. A resource can have multiple themes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>dcat:themeTaxonomy</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>dcat:Catalog</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>rdfs:Resource</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>theme taxonomy</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>The knowledge organization system (KOS) used to classify catalog's datasets.</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>dcat:version</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>The version indicator (name or identifier) of a resource.</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>foaf:homepage</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>This axiom needed so that Protege loads DCAT 3 without errors.</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>foaf:primaryTopic</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr"/>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>This axiom needed so that Protege loads DCAT 3 without errors.</t>
         </is>
       </c>
     </row>

</xml_diff>